<commit_message>
Debug user input logical errors
</commit_message>
<xml_diff>
--- a/empty.xlsx
+++ b/empty.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>H</t>
   </si>
@@ -22,88 +22,91 @@
     <t>K</t>
   </si>
   <si>
-    <t>03:00</t>
+    <t>03:30</t>
   </si>
   <si>
     <t>05:30</t>
   </si>
   <si>
-    <t>07:00</t>
-  </si>
-  <si>
-    <t>09:00</t>
+    <t>09:30</t>
   </si>
   <si>
     <t>10:00</t>
   </si>
   <si>
-    <t>11:15</t>
+    <t>10:45</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>12:30</t>
+  </si>
+  <si>
+    <t>15:45</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>18:30</t>
+  </si>
+  <si>
+    <t>19:15</t>
+  </si>
+  <si>
+    <t>19:45</t>
+  </si>
+  <si>
+    <t>ΕΛΕΝΗ</t>
+  </si>
+  <si>
+    <t>ΙΩΝΑΣ</t>
+  </si>
+  <si>
+    <t>ΝΑΝΤΗ</t>
+  </si>
+  <si>
+    <t>ΕΡΜΗΣ</t>
+  </si>
+  <si>
+    <t>ΑΓΙΑ ΕΙΡΗΝΗ</t>
+  </si>
+  <si>
+    <t>ΑΓΙΟΣ ΣΠΥΡΙΔΩΝ</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>07:30</t>
+  </si>
+  <si>
+    <t>08:45</t>
+  </si>
+  <si>
+    <t>10:30</t>
+  </si>
+  <si>
+    <t>12:15</t>
   </si>
   <si>
     <t>13:00</t>
   </si>
   <si>
-    <t>14:15</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>16:15</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>19:15</t>
-  </si>
-  <si>
-    <t>20:15</t>
-  </si>
-  <si>
-    <t>ΕΛΕΝΗ</t>
-  </si>
-  <si>
-    <t>ΙΩΝΑΣ</t>
-  </si>
-  <si>
-    <t>ΑΓΙΟΣ ΣΠΥΡΙΔΩΝ</t>
-  </si>
-  <si>
-    <t>ΑΓΙΑ ΕΙΡΗΝΗ</t>
-  </si>
-  <si>
-    <t>ΕΡΜΗΣ</t>
-  </si>
-  <si>
-    <t>ΝΑΝΤΗ</t>
-  </si>
-  <si>
-    <t>07:30</t>
-  </si>
-  <si>
-    <t>09:15</t>
-  </si>
-  <si>
-    <t>11:45</t>
-  </si>
-  <si>
-    <t>12:45</t>
-  </si>
-  <si>
-    <t>13:30</t>
-  </si>
-  <si>
-    <t>15:30</t>
+    <t>13:45</t>
+  </si>
+  <si>
+    <t>14:45</t>
   </si>
   <si>
     <t>17:00</t>
   </si>
   <si>
-    <t>18:15</t>
-  </si>
-  <si>
-    <t>23:30</t>
+    <t>17:45</t>
+  </si>
+  <si>
+    <t>20:45</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -482,13 +485,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -496,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -510,13 +513,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -524,13 +527,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -538,13 +541,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -552,13 +555,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -566,13 +569,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -580,13 +583,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -594,13 +597,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -611,7 +614,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -622,10 +625,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
@@ -636,27 +639,13 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>